<commit_message>
Add technical details overview
</commit_message>
<xml_diff>
--- a/hamilton-thermostat-main-BOM.xlsx
+++ b/hamilton-thermostat-main-BOM.xlsx
@@ -294,18 +294,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>AT24CM01 (or AT24CM02)</t>
-  </si>
-  <si>
-    <t>AT24CM01-XHM-TTR-ND</t>
-  </si>
-  <si>
-    <t>1Mbit (or 2Mbit) EEPROM</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/microchip-technology/AT24CM01-XHM-T/AT24CM01-XHM-TTR-ND/3913189</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
@@ -787,13 +775,25 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/nexperia-usa-inc/IP4220CZ6,125/1727-3578-1-ND/1133548</t>
+  </si>
+  <si>
+    <t>AT24CM02</t>
+  </si>
+  <si>
+    <t>2Mbit EEPROM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/AT24CM02-SSHD-B/AT24CM02-SSHD-B-ND/5313448</t>
+  </si>
+  <si>
+    <t>AT24CM02-SSHD-B-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -804,6 +804,19 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -827,11 +840,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1149,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1217,10 +1231,10 @@
       <c r="H2" s="1">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1241,10 +1255,10 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1271,10 +1285,10 @@
       <c r="H4" s="1">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1303,10 +1317,10 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1333,10 +1347,10 @@
       <c r="H6" s="1">
         <v>6</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1365,8 +1379,8 @@
       <c r="H7" s="1">
         <v>4</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1395,10 +1409,10 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1425,10 +1439,10 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1455,10 +1469,10 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1485,10 +1499,10 @@
       <c r="H11" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1517,10 +1531,10 @@
       <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J12" s="3"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1547,10 +1561,10 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="3"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1574,10 +1588,10 @@
       <c r="H14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J14" s="3"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1604,23 +1618,23 @@
       <c r="H15" s="1">
         <v>1</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>92</v>
+        <v>252</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>93</v>
+        <v>253</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>88</v>
@@ -1634,23 +1648,23 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="3"/>
+      <c r="I16" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>47</v>
@@ -1664,26 +1678,26 @@
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="3"/>
+      <c r="I17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="F18" s="1">
         <v>0.12128</v>
@@ -1694,26 +1708,26 @@
       <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="J18" s="3"/>
+      <c r="I18" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F19" s="1">
         <v>2.7048000000000001</v>
@@ -1724,26 +1738,26 @@
       <c r="H19" s="1">
         <v>1</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J19" s="3"/>
+      <c r="I19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="F20" s="1">
         <v>0.63963000000000003</v>
@@ -1754,28 +1768,28 @@
       <c r="H20" s="1">
         <v>1</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>112</v>
+      <c r="I20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="F21" s="1">
         <v>0.50749999999999995</v>
@@ -1786,26 +1800,26 @@
       <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J21" s="3"/>
+      <c r="I21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F22" s="1">
         <v>0.495</v>
@@ -1816,26 +1830,26 @@
       <c r="H22" s="1">
         <v>1</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" s="3"/>
+      <c r="I22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="F23" s="1">
         <v>0.64515</v>
@@ -1846,26 +1860,26 @@
       <c r="H23" s="1">
         <v>1</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J23" s="3"/>
+      <c r="I23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F24" s="1">
         <v>0.56694999999999995</v>
@@ -1876,26 +1890,26 @@
       <c r="H24" s="1">
         <v>1</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J24" s="3"/>
+      <c r="I24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="F25" s="1">
         <v>0.41344999999999998</v>
@@ -1906,26 +1920,26 @@
       <c r="H25" s="1">
         <v>1</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J25" s="3"/>
+      <c r="I25" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="F26" s="1">
         <v>2.2849999999999999E-2</v>
@@ -1936,23 +1950,23 @@
       <c r="H26" s="1">
         <v>1</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J26" s="3"/>
+      <c r="I26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>29</v>
@@ -1966,26 +1980,26 @@
       <c r="H27" s="1">
         <v>1</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J27" s="3"/>
+      <c r="I27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="F28" s="1">
         <v>0.3296</v>
@@ -1996,26 +2010,26 @@
       <c r="H28" s="1">
         <v>1</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J28" s="3"/>
+      <c r="I28" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F29" s="1">
         <v>6.1500000000000001E-3</v>
@@ -2026,26 +2040,26 @@
       <c r="H29" s="1">
         <v>4</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="J29" s="3"/>
+      <c r="I29" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F30" s="1">
         <v>2.545E-2</v>
@@ -2056,26 +2070,26 @@
       <c r="H30" s="1">
         <v>1</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J30" s="3"/>
+      <c r="I30" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F31" s="1">
         <v>2.1819999999999999E-2</v>
@@ -2086,26 +2100,26 @@
       <c r="H31" s="1">
         <v>1</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="J31" s="3"/>
+      <c r="I31" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F32" s="1">
         <v>0.40365000000000001</v>
@@ -2116,26 +2130,26 @@
       <c r="H32" s="1">
         <v>1</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="J32" s="3"/>
+      <c r="I32" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F33" s="1">
         <v>1.9189999999999999E-2</v>
@@ -2146,26 +2160,26 @@
       <c r="H33" s="1">
         <v>1</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="J33" s="3"/>
+      <c r="I33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F34" s="1">
         <v>6.1500000000000001E-3</v>
@@ -2176,26 +2190,26 @@
       <c r="H34" s="1">
         <v>2</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J34" s="3"/>
+      <c r="I34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="F35" s="1">
         <v>0.11475</v>
@@ -2206,26 +2220,26 @@
       <c r="H35" s="1">
         <v>1</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3" t="s">
-        <v>189</v>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="F36" s="1">
         <v>0.10659</v>
@@ -2236,26 +2250,26 @@
       <c r="H36" s="1">
         <v>1</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3" t="s">
-        <v>195</v>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F37" s="1">
         <v>3.3999999999999998E-3</v>
@@ -2266,26 +2280,26 @@
       <c r="H37" s="1">
         <v>1</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="J37" s="3"/>
+      <c r="I37" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="F38" s="1">
         <v>4.3</v>
@@ -2296,28 +2310,28 @@
       <c r="H38" s="1">
         <v>1</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>207</v>
+      <c r="I38" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B39" s="1">
         <v>1935200</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F39" s="1">
         <v>0.82450000000000001</v>
@@ -2328,26 +2342,26 @@
       <c r="H39" s="1">
         <v>1</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="J39" s="3"/>
+      <c r="I39" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F40" s="1">
         <v>0.67430999999999996</v>
@@ -2358,35 +2372,35 @@
       <c r="H40" s="1">
         <v>1</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="J40" s="3"/>
+      <c r="I40" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+        <v>215</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
       <c r="F44" s="1">
         <v>3.3899999999999998E-3</v>
       </c>
@@ -2396,18 +2410,18 @@
       <c r="H44" s="1">
         <v>2</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
       <c r="F45" s="1">
         <v>2.16E-3</v>
       </c>
@@ -2417,18 +2431,18 @@
       <c r="H45" s="1">
         <v>7</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
       <c r="F46" s="1">
         <v>5.7499999999999999E-3</v>
       </c>
@@ -2438,18 +2452,18 @@
       <c r="H46" s="1">
         <v>4</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
       <c r="F47" s="1">
         <v>1.91E-3</v>
       </c>
@@ -2459,18 +2473,18 @@
       <c r="H47" s="1">
         <v>2</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
       <c r="F48" s="1">
         <v>2.9170000000000001E-2</v>
       </c>
@@ -2480,20 +2494,20 @@
       <c r="H48" s="1">
         <v>2</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="J48" s="3"/>
+      <c r="I48" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+        <v>226</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
       <c r="F49" s="1">
         <v>1.2099999999999999E-3</v>
       </c>
@@ -2503,18 +2517,18 @@
       <c r="H49" s="1">
         <v>7</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
       <c r="F50" s="1">
         <v>1.2099999999999999E-3</v>
       </c>
@@ -2524,22 +2538,22 @@
       <c r="H50" s="1">
         <v>6</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>235</v>
+      <c r="I50" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+        <v>232</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
       <c r="F51" s="1">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -2549,65 +2563,65 @@
       <c r="H51" s="1">
         <v>2</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="J51" s="3"/>
+      <c r="I51" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J51" s="2"/>
     </row>
     <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
     </row>
     <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
     </row>
     <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
+        <v>235</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
     </row>
     <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="J55" s="3"/>
+        <v>238</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J55" s="2"/>
     </row>
     <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="J56" s="3"/>
+        <v>242</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -3605,40 +3619,39 @@
     <hyperlink ref="I13" r:id="rId15"/>
     <hyperlink ref="I14" r:id="rId16"/>
     <hyperlink ref="I15" r:id="rId17"/>
-    <hyperlink ref="I16" r:id="rId18"/>
-    <hyperlink ref="I17" r:id="rId19"/>
-    <hyperlink ref="I19" r:id="rId20"/>
-    <hyperlink ref="I20" r:id="rId21"/>
-    <hyperlink ref="J20" r:id="rId22"/>
-    <hyperlink ref="I21" r:id="rId23"/>
-    <hyperlink ref="I22" r:id="rId24"/>
-    <hyperlink ref="I23" r:id="rId25"/>
-    <hyperlink ref="I24" r:id="rId26"/>
-    <hyperlink ref="I25" r:id="rId27"/>
-    <hyperlink ref="I26" r:id="rId28"/>
-    <hyperlink ref="I27" r:id="rId29"/>
-    <hyperlink ref="I28" r:id="rId30"/>
-    <hyperlink ref="I29" r:id="rId31"/>
-    <hyperlink ref="I30" r:id="rId32"/>
-    <hyperlink ref="I31" r:id="rId33"/>
-    <hyperlink ref="I32" r:id="rId34"/>
-    <hyperlink ref="I33" r:id="rId35"/>
-    <hyperlink ref="I34" r:id="rId36"/>
-    <hyperlink ref="J35" r:id="rId37"/>
-    <hyperlink ref="J36" r:id="rId38"/>
-    <hyperlink ref="I37" r:id="rId39"/>
-    <hyperlink ref="I38" r:id="rId40"/>
-    <hyperlink ref="J38" r:id="rId41"/>
-    <hyperlink ref="I39" r:id="rId42"/>
-    <hyperlink ref="I40" r:id="rId43"/>
-    <hyperlink ref="I48" r:id="rId44"/>
-    <hyperlink ref="I50" r:id="rId45"/>
-    <hyperlink ref="J50" r:id="rId46"/>
-    <hyperlink ref="I51" r:id="rId47"/>
-    <hyperlink ref="I55" r:id="rId48"/>
-    <hyperlink ref="I56" r:id="rId49"/>
+    <hyperlink ref="I17" r:id="rId18"/>
+    <hyperlink ref="I19" r:id="rId19"/>
+    <hyperlink ref="I20" r:id="rId20"/>
+    <hyperlink ref="J20" r:id="rId21"/>
+    <hyperlink ref="I21" r:id="rId22"/>
+    <hyperlink ref="I22" r:id="rId23"/>
+    <hyperlink ref="I23" r:id="rId24"/>
+    <hyperlink ref="I24" r:id="rId25"/>
+    <hyperlink ref="I25" r:id="rId26"/>
+    <hyperlink ref="I26" r:id="rId27"/>
+    <hyperlink ref="I27" r:id="rId28"/>
+    <hyperlink ref="I28" r:id="rId29"/>
+    <hyperlink ref="I29" r:id="rId30"/>
+    <hyperlink ref="I30" r:id="rId31"/>
+    <hyperlink ref="I31" r:id="rId32"/>
+    <hyperlink ref="I32" r:id="rId33"/>
+    <hyperlink ref="I33" r:id="rId34"/>
+    <hyperlink ref="I34" r:id="rId35"/>
+    <hyperlink ref="J35" r:id="rId36"/>
+    <hyperlink ref="J36" r:id="rId37"/>
+    <hyperlink ref="I37" r:id="rId38"/>
+    <hyperlink ref="I38" r:id="rId39"/>
+    <hyperlink ref="J38" r:id="rId40"/>
+    <hyperlink ref="I39" r:id="rId41"/>
+    <hyperlink ref="I40" r:id="rId42"/>
+    <hyperlink ref="I48" r:id="rId43"/>
+    <hyperlink ref="I50" r:id="rId44"/>
+    <hyperlink ref="J50" r:id="rId45"/>
+    <hyperlink ref="I51" r:id="rId46"/>
+    <hyperlink ref="I55" r:id="rId47"/>
+    <hyperlink ref="I56" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>